<commit_message>
Dashboard control and feedback working
</commit_message>
<xml_diff>
--- a/Version 2/BOM.xlsx
+++ b/Version 2/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fairbanksgov-my.sharepoint.us/personal/john_steagall_fairbanksmorse_com/Documents/Documents/GitHub/FMTDev/Version 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DF875AA-35A8-447A-8DB5-FC5D7E9FF90A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{3DF875AA-35A8-447A-8DB5-FC5D7E9FF90A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{575788F9-1CCD-4D1D-9D4B-F4B3F619DF00}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="192">
   <si>
     <t>Battery</t>
   </si>
@@ -576,6 +576,42 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/chip-quik-inc/SMD291SNL/1160001</t>
+  </si>
+  <si>
+    <t>TEMP1</t>
+  </si>
+  <si>
+    <t>TEMP2</t>
+  </si>
+  <si>
+    <t>TEMP3</t>
+  </si>
+  <si>
+    <t>LM335Z</t>
+  </si>
+  <si>
+    <t>SENSOR ANALOG -40C-100C TO92-3</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stmicroelectronics/LM335Z/591686?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Supplier_STMicroelectronics&amp;utm_term=&amp;utm_content=General&amp;gclid=Cj0KCQiAw8OeBhCeARIsAGxWtUywoYtO5LAvKE5V4JY6vC32rmQtlLVKhOjiFkYAQxgWaDaNm1yvAgwaArL5EALw_wcB</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Superele-Precision-Centigrade-Temperature-Sensors/dp/B01NAPD79A?source=ps-sl-shoppingads-lpcontext&amp;ref_=fplfs&amp;psc=1&amp;smid=AI3KZT5ZPMWVT</t>
+  </si>
+  <si>
+    <t>Temp1</t>
+  </si>
+  <si>
+    <t>Temp2</t>
+  </si>
+  <si>
+    <t>Temp3</t>
+  </si>
+  <si>
+    <t>LM35DZ</t>
+  </si>
+  <si>
+    <t>LM35 LM35DZ TO92 TO-92 Precision Centigrade Temperature Sensors</t>
   </si>
 </sst>
 </file>
@@ -647,7 +683,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -656,6 +692,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1012,10 +1049,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4879CCF8-B0FD-4E88-A6F2-08E6030602D0}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K68"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1287,7 +1324,7 @@
       <c r="C10" t="s">
         <v>43</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E10" t="s">
@@ -2140,7 +2177,7 @@
         <v>1</v>
       </c>
       <c r="H43">
-        <f t="shared" ref="H43:H64" si="1">IF(I43="Yes",0,G43*F43)</f>
+        <f t="shared" ref="H43:H70" si="1">IF(I43="Yes",0,G43*F43)</f>
         <v>0.79</v>
       </c>
       <c r="I43" t="s">
@@ -2741,10 +2778,172 @@
         <v>29</v>
       </c>
     </row>
-    <row r="68" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>180</v>
+      </c>
+      <c r="B65" t="s">
+        <v>183</v>
+      </c>
+      <c r="C65" t="s">
+        <v>184</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F65">
+        <v>0.69</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="1"/>
+        <v>0.69</v>
+      </c>
+      <c r="I65" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>181</v>
+      </c>
+      <c r="B66" t="s">
+        <v>183</v>
+      </c>
+      <c r="C66" t="s">
+        <v>184</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F66">
+        <v>0.69</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="1"/>
+        <v>0.69</v>
+      </c>
+      <c r="I66" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>182</v>
+      </c>
+      <c r="B67" t="s">
+        <v>183</v>
+      </c>
+      <c r="C67" t="s">
+        <v>184</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F67">
+        <v>0.69</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="1"/>
+        <v>0.69</v>
+      </c>
+      <c r="I67" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>187</v>
+      </c>
+      <c r="B68" t="s">
+        <v>190</v>
+      </c>
+      <c r="C68" t="s">
+        <v>191</v>
+      </c>
+      <c r="D68" t="s">
+        <v>186</v>
+      </c>
+      <c r="F68">
+        <v>26.99</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
       <c r="H68">
-        <f>SUM(H2:H67)</f>
-        <v>1036.03</v>
+        <f t="shared" si="1"/>
+        <v>26.99</v>
+      </c>
+      <c r="I68" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>188</v>
+      </c>
+      <c r="B69" t="s">
+        <v>190</v>
+      </c>
+      <c r="C69" t="s">
+        <v>191</v>
+      </c>
+      <c r="D69" t="s">
+        <v>186</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I69" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>189</v>
+      </c>
+      <c r="B70" t="s">
+        <v>190</v>
+      </c>
+      <c r="C70" t="s">
+        <v>191</v>
+      </c>
+      <c r="D70" t="s">
+        <v>186</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I70" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H76">
+        <f>SUM(H2:H70)</f>
+        <v>1065.0900000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2769,9 +2968,10 @@
     <hyperlink ref="D58:D61" r:id="rId11" display="https://www.dfrobot.com/product-2130.html" xr:uid="{E9BE7256-0752-4363-9156-02EAF2D4A079}"/>
     <hyperlink ref="D63:D64" r:id="rId12" display="https://store.opencv.ai/products/oak-d" xr:uid="{8C9769E1-4919-48FB-9308-D051E226934A}"/>
     <hyperlink ref="A54" r:id="rId13" display="CON@" xr:uid="{429327F3-446B-4320-854B-1E54ABB9B033}"/>
+    <hyperlink ref="D10" r:id="rId14" display="https://www.digikey.com/en/products/detail/sanyo-denki-america-inc./109P0624W601/6191895?utm_adgroup=SANYO%20DENKI%20AMERICA%20INC.&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_DK%2BSupplier_Tier%203%20-%20Block%202&amp;utm_term=&amp;utm_content=SANYO%20DENKI%20AMERICA%20INC.&amp;gclid=CjwKCAiAzp6eBhByEiwA_gGq5HysfpQclofZjwac-D9ERxLfewmzafxfYBqHexqLbLN8lqw0JwGCZRoCrawQAvD_BwE" xr:uid="{0F329E82-9FF8-443B-BE88-49A3D007BAEE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId14"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId15"/>
 </worksheet>
 </file>
 
@@ -2960,29 +3160,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <FileHash xmlns="23f8a761-462b-40aa-8754-dc239dce3ff2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="23f8a761-462b-40aa-8754-dc239dce3ff2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="30f68630-5399-4187-9335-db3767ff873b" xsi:nil="true"/>
-    <UniqueSourceRef xmlns="23f8a761-462b-40aa-8754-dc239dce3ff2" xsi:nil="true"/>
-    <CloudMigratorVersion xmlns="23f8a761-462b-40aa-8754-dc239dce3ff2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009EB4A01376AD7741A349CF90BEEE7BA2" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="40011c4354fad08aa6c8105627212889">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="23f8a761-462b-40aa-8754-dc239dce3ff2" xmlns:ns3="30f68630-5399-4187-9335-db3767ff873b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a571f3f1f810c9f297ea861c19d93485" ns2:_="" ns3:_="">
     <xsd:import namespace="23f8a761-462b-40aa-8754-dc239dce3ff2"/>
@@ -3229,26 +3406,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF01283E-90BF-4FD6-BB30-1115D8730D47}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="23f8a761-462b-40aa-8754-dc239dce3ff2"/>
-    <ds:schemaRef ds:uri="30f68630-5399-4187-9335-db3767ff873b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16EDBB8A-7086-4225-817D-E0A3609B9346}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <FileHash xmlns="23f8a761-462b-40aa-8754-dc239dce3ff2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="23f8a761-462b-40aa-8754-dc239dce3ff2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="30f68630-5399-4187-9335-db3767ff873b" xsi:nil="true"/>
+    <UniqueSourceRef xmlns="23f8a761-462b-40aa-8754-dc239dce3ff2" xsi:nil="true"/>
+    <CloudMigratorVersion xmlns="23f8a761-462b-40aa-8754-dc239dce3ff2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2B00FC5-2499-46A4-8616-D8364262A769}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3265,4 +3446,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16EDBB8A-7086-4225-817D-E0A3609B9346}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF01283E-90BF-4FD6-BB30-1115D8730D47}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="23f8a761-462b-40aa-8754-dc239dce3ff2"/>
+    <ds:schemaRef ds:uri="30f68630-5399-4187-9335-db3767ff873b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>